<commit_message>
Updated template and Jhpiego example.
</commit_message>
<xml_diff>
--- a/Templates/PCI modele 2015-07-27.xlsx
+++ b/Templates/PCI modele 2015-07-27.xlsx
@@ -8,12 +8,12 @@
   </bookViews>
   <sheets>
     <sheet name="Rapport" sheetId="2" r:id="rId1"/>
-    <sheet name="Regions" sheetId="5" r:id="rId2"/>
-    <sheet name="Prefectures" sheetId="6" r:id="rId3"/>
-    <sheet name="Sous-prefectures" sheetId="7" r:id="rId4"/>
-    <sheet name="Etablissements" sheetId="10" r:id="rId5"/>
-    <sheet name="Partenaires" sheetId="3" r:id="rId6"/>
-    <sheet name="Types" sheetId="4" r:id="rId7"/>
+    <sheet name="Regions" sheetId="5" state="hidden" r:id="rId2"/>
+    <sheet name="Prefectures" sheetId="6" state="hidden" r:id="rId3"/>
+    <sheet name="Sous-prefectures" sheetId="7" state="hidden" r:id="rId4"/>
+    <sheet name="Etablissements" sheetId="10" state="hidden" r:id="rId5"/>
+    <sheet name="Partenaires" sheetId="3" state="hidden" r:id="rId6"/>
+    <sheet name="Types" sheetId="4" state="hidden" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="FacilityKey">Etablissements!$A$2</definedName>
@@ -28,54 +28,6 @@
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
-</file>
-
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="facilities-pcoded1" type="6" refreshedVersion="3" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="E:\gin-master-facilities\facilities-pcoded.csv" tab="0" comma="1">
-      <textFields count="7">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="2" name="prefectures" type="6" refreshedVersion="3" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="E:\gin-master-facilities\prefectures.csv" tab="0" comma="1">
-      <textFields count="4">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="3" name="regions" type="6" refreshedVersion="3" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="E:\gin-master-facilities\regions.csv" tab="0" comma="1">
-      <textFields count="2">
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="4" name="subprefectures" type="6" refreshedVersion="3" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="E:\gin-master-facilities\subprefectures.csv" tab="0" comma="1">
-      <textFields count="6">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6406,7 +6358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6454,15 +6406,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6485,7 +6428,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6795,104 +6745,103 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.42578125" style="17"/>
-    <col min="7" max="7" width="22.85546875" style="17" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="17"/>
+    <col min="1" max="2" width="15.7109375" style="26" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="26" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="26" customWidth="1"/>
+    <col min="5" max="6" width="12.7109375" style="26" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="26" customWidth="1"/>
+    <col min="8" max="11" width="12.7109375" style="26" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="18" customFormat="1" ht="21" customHeight="1">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:11" s="25" customFormat="1" ht="21" customHeight="1">
+      <c r="A1" s="22" t="s">
         <v>2062</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="27" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="24" t="s">
         <v>1576</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-    </row>
-    <row r="2" spans="1:11" s="18" customFormat="1" ht="65.25" customHeight="1">
-      <c r="A2" s="19" t="s">
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+    </row>
+    <row r="2" spans="1:11" s="25" customFormat="1" ht="65.25" customHeight="1">
+      <c r="A2" s="17" t="s">
         <v>1577</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>1574</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="17" t="s">
         <v>1575</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="17" t="s">
         <v>2063</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="17" t="s">
         <v>1578</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="17" t="s">
         <v>2064</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="18" t="s">
         <v>2061</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="18" t="s">
         <v>1579</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="18" t="s">
         <v>1580</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="18" t="s">
         <v>1606</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="18" t="s">
         <v>1581</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="24" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:11" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="A3" s="19" t="s">
         <v>1582</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="19" t="s">
         <v>1583</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>1584</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="19" t="s">
         <v>1585</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="19" t="s">
         <v>1586</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="19" t="s">
         <v>1587</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="20" t="s">
         <v>2036</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="20" t="s">
         <v>1591</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="20" t="s">
         <v>1592</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="20" t="s">
         <v>1593</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="20" t="s">
         <v>1594</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:K1"/>
@@ -6915,16 +6864,16 @@
     <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Date inacceptable" error="S'il vous plaît spécifier une date après le 1er Janvier 2015." promptTitle="Date" prompt="La date quand la formation a ete completee." sqref="H4:H4000">
       <formula1>42005</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Région" prompt="La région où se situe l'établissement." sqref="A4:A4000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Région" prompt="Dans le menu, choisissez la région où se situe l'établissement." sqref="A4:A4000">
       <formula1>Regions</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Préfecture" prompt="La préfecture où se situe l'établissement (choissez d'abord la région)." sqref="B4:B4000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Préfecture" prompt="Dans le menu, choisissez la préfecture où se situe l'établissement (choisissez d'abord la région)." sqref="B4:B4000">
       <formula1>OFFSET(PrefectureKey,MATCH(A4,PrefectureRegions,0),0,COUNTIF(PrefectureRegions,A4), 1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sous-préfecture" prompt="La sous-préfecture où se situe l'établissement (choissez d'abord la région et la préfecture)." sqref="C4:C4000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Sous-préfecture" prompt="Dans le menu, choisissez la sous-préfecture où se situe l'établissement (choisissez d'abord la région et la préfecture)." sqref="C4:C4000">
       <formula1>OFFSET(SubprefectureKey,MATCH(B4,SubprefecturePrefectures,0),0,COUNTIF(SubprefecturePrefectures,B4), 1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Nom de l'établissement" prompt="Choissez d'abord la région, la préfecture, et la sous-préfecture._x000a__x000a_Si l'établissement ne figure pas dans la liste, s'il vous plaît taper son nom." sqref="D4:D4000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Nom de l'établissement" prompt="Dans le menu, choisissez le nom de l'établissement (choisissez d'abord la région, la préfecture, et la sous-préfecture)._x000a__x000a_Si l'établissement ne figure pas dans la liste, s'il vous plaît taper son nom." sqref="D4:D4000">
       <formula1>OFFSET(FacilityKey,MATCH(C4,FacilitySubprefectures,0),0,COUNTIF(FacilitySubprefectures,C4), 1)</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Numéro invalide" error="Spécifier le nombre total de personnel de l'établissement (au moins 1)." promptTitle="Total du personnel" prompt="Nombre de tout le personnel de l'établissement, y compris ceux qui ne l'ont pas été formés." sqref="E4:E4000">
@@ -6946,7 +6895,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7051,7 +7000,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7582,7 +7531,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14451,7 +14400,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44386,7 +44335,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A4"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -44553,7 +44502,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>